<commit_message>
Versión 2.2 multithreading activado
</commit_message>
<xml_diff>
--- a/andina-maxiconsumo-ACTUALIZADO.xlsx
+++ b/andina-maxiconsumo-ACTUALIZADO.xlsx
@@ -505,7 +505,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$ 2.479,26</t>
+          <t>$ 2.776,77</t>
         </is>
       </c>
     </row>
@@ -533,7 +533,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$ 1.239,59</t>
+          <t>$ 1.295,77</t>
         </is>
       </c>
     </row>
@@ -617,7 +617,7 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$ 1.404,87</t>
+          <t>$ 1.573,45</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$ 1.404,87</t>
+          <t>$ 1.573,45</t>
         </is>
       </c>
     </row>
@@ -673,7 +673,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>$ 1.404,87</t>
+          <t>$ 1.573,45</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$ 1.074,29</t>
+          <t>$ 1.203,20</t>
         </is>
       </c>
     </row>
@@ -757,7 +757,7 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>$ 561,90</t>
+          <t>$ 629,33</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>$ 1.652,81</t>
+          <t>$ 2.036,26</t>
         </is>
       </c>
     </row>

</xml_diff>